<commit_message>
Añadi campos nuevos a la tabla usuario, subi 3 sp y actualice el cronograma
</commit_message>
<xml_diff>
--- a/desarrollo/SW_ModeloDeCalidad-ISO9126/7. Gestión/Cronograma GCM.xlsx
+++ b/desarrollo/SW_ModeloDeCalidad-ISO9126/7. Gestión/Cronograma GCM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
   <si>
     <t>Nombre del proyecto</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>El sistema elaborará un reporte de la lista de métricas priorizadas para que el usuario las tome en cuenta en el desarrollo de su proyecto</t>
+  </si>
+  <si>
+    <t>En progreso</t>
   </si>
 </sst>
 </file>
@@ -225,7 +228,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,8 +265,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,6 +307,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFC0202"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -472,7 +488,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -615,6 +631,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -908,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,7 +991,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="12">
-        <v>0.01</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="8" spans="2:40" ht="30" x14ac:dyDescent="0.25">
@@ -1907,9 +1929,11 @@
       <c r="F27">
         <v>3</v>
       </c>
-      <c r="G27" s="63"/>
-      <c r="H27" s="19">
-        <v>0</v>
+      <c r="G27" s="72" t="s">
+        <v>64</v>
+      </c>
+      <c r="H27" s="71">
+        <v>0.8</v>
       </c>
       <c r="I27" s="32"/>
       <c r="J27" s="32"/>
@@ -1938,23 +1962,25 @@
     </row>
     <row r="28" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B28" s="24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D28" s="14">
-        <v>44044</v>
+        <v>44037</v>
       </c>
       <c r="E28" s="30">
-        <v>44046</v>
+        <v>44038</v>
       </c>
       <c r="F28">
-        <v>3</v>
-      </c>
-      <c r="G28" s="64"/>
-      <c r="H28" s="19">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="G28" s="62" t="s">
+        <v>55</v>
+      </c>
+      <c r="H28" s="37">
+        <v>1</v>
       </c>
       <c r="I28" s="32"/>
       <c r="J28" s="32"/>
@@ -1969,10 +1995,10 @@
       <c r="S28" s="32"/>
       <c r="T28" s="32"/>
       <c r="U28" s="32"/>
-      <c r="V28" s="32"/>
+      <c r="V28" s="67"/>
       <c r="W28" s="32"/>
-      <c r="X28" s="67"/>
-      <c r="Y28" s="67"/>
+      <c r="X28" s="32"/>
+      <c r="Z28" s="32"/>
       <c r="AA28" s="32"/>
       <c r="AB28" s="32"/>
       <c r="AC28" s="32"/>
@@ -1983,23 +2009,25 @@
     </row>
     <row r="29" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B29" s="24" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D29" s="14">
         <v>44037</v>
       </c>
       <c r="E29" s="30">
-        <v>44038</v>
+        <v>44040</v>
       </c>
       <c r="F29">
-        <v>2</v>
-      </c>
-      <c r="G29" s="64"/>
-      <c r="H29" s="19">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="G29" s="62" t="s">
+        <v>55</v>
+      </c>
+      <c r="H29" s="37">
+        <v>1</v>
       </c>
       <c r="I29" s="32"/>
       <c r="J29" s="32"/>
@@ -2015,8 +2043,9 @@
       <c r="T29" s="32"/>
       <c r="U29" s="32"/>
       <c r="V29" s="67"/>
-      <c r="W29" s="32"/>
-      <c r="X29" s="32"/>
+      <c r="W29" s="67"/>
+      <c r="X29" s="68"/>
+      <c r="Y29" s="32"/>
       <c r="Z29" s="32"/>
       <c r="AA29" s="32"/>
       <c r="AB29" s="32"/>
@@ -2028,19 +2057,19 @@
     </row>
     <row r="30" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B30" s="24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D30" s="14">
+        <v>44044</v>
+      </c>
+      <c r="E30" s="30">
         <v>44046</v>
       </c>
-      <c r="E30" s="30">
-        <v>44047</v>
-      </c>
       <c r="F30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G30" s="64"/>
       <c r="H30" s="19">
@@ -2061,11 +2090,11 @@
       <c r="U30" s="32"/>
       <c r="V30" s="32"/>
       <c r="W30" s="32"/>
-      <c r="X30" s="32"/>
+      <c r="X30" s="67"/>
       <c r="Y30" s="67"/>
-      <c r="Z30" s="32"/>
       <c r="AA30" s="32"/>
       <c r="AB30" s="32"/>
+      <c r="AC30" s="32"/>
       <c r="AD30" s="32"/>
       <c r="AE30" s="32"/>
       <c r="AF30" s="32"/>
@@ -2073,19 +2102,19 @@
     </row>
     <row r="31" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B31" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D31" s="14">
-        <v>44037</v>
+        <v>44046</v>
       </c>
       <c r="E31" s="30">
-        <v>44040</v>
+        <v>44047</v>
       </c>
       <c r="F31">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G31" s="64"/>
       <c r="H31" s="19">
@@ -2104,9 +2133,10 @@
       <c r="S31" s="32"/>
       <c r="T31" s="32"/>
       <c r="U31" s="32"/>
-      <c r="V31" s="67"/>
-      <c r="W31" s="67"/>
-      <c r="X31" s="68"/>
+      <c r="V31" s="32"/>
+      <c r="W31" s="32"/>
+      <c r="X31" s="32"/>
+      <c r="Y31" s="67"/>
       <c r="Z31" s="32"/>
       <c r="AA31" s="32"/>
       <c r="AB31" s="32"/>
@@ -2378,19 +2408,19 @@
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B38" s="21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D38" s="42">
-        <v>44062</v>
+        <v>44058</v>
       </c>
       <c r="E38" s="54">
-        <v>44064</v>
+        <v>44059</v>
       </c>
       <c r="F38" s="49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G38" s="64"/>
       <c r="H38" s="50">
@@ -2416,27 +2446,27 @@
       <c r="Z38" s="32"/>
       <c r="AA38" s="32"/>
       <c r="AB38" s="32"/>
-      <c r="AC38" s="32"/>
-      <c r="AD38" s="67"/>
-      <c r="AE38" s="67"/>
+      <c r="AC38" s="67"/>
+      <c r="AD38" s="32"/>
+      <c r="AE38" s="32"/>
       <c r="AF38" s="32"/>
       <c r="AG38" s="32"/>
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B39" s="21" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D39" s="42">
         <v>44058</v>
       </c>
       <c r="E39" s="54">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="F39" s="49">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G39" s="64"/>
       <c r="H39" s="50">
@@ -2463,26 +2493,26 @@
       <c r="AA39" s="32"/>
       <c r="AB39" s="32"/>
       <c r="AC39" s="67"/>
-      <c r="AD39" s="32"/>
+      <c r="AD39" s="67"/>
       <c r="AE39" s="32"/>
       <c r="AF39" s="32"/>
       <c r="AG39" s="32"/>
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B40" s="21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D40" s="42">
+        <v>44062</v>
+      </c>
+      <c r="E40" s="54">
         <v>44064</v>
       </c>
-      <c r="E40" s="54">
-        <v>44065</v>
-      </c>
       <c r="F40" s="49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G40" s="64"/>
       <c r="H40" s="50">
@@ -2509,26 +2539,26 @@
       <c r="AA40" s="32"/>
       <c r="AB40" s="32"/>
       <c r="AC40" s="32"/>
-      <c r="AD40" s="32"/>
+      <c r="AD40" s="67"/>
       <c r="AE40" s="67"/>
       <c r="AF40" s="32"/>
       <c r="AG40" s="32"/>
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B41" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D41" s="42">
-        <v>44058</v>
+        <v>44064</v>
       </c>
       <c r="E41" s="54">
-        <v>44061</v>
+        <v>44065</v>
       </c>
       <c r="F41" s="49">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G41" s="64"/>
       <c r="H41" s="50">
@@ -2554,9 +2584,9 @@
       <c r="Z41" s="32"/>
       <c r="AA41" s="32"/>
       <c r="AB41" s="32"/>
-      <c r="AC41" s="67"/>
-      <c r="AD41" s="67"/>
-      <c r="AE41" s="32"/>
+      <c r="AC41" s="32"/>
+      <c r="AD41" s="32"/>
+      <c r="AE41" s="67"/>
       <c r="AF41" s="32"/>
       <c r="AG41" s="32"/>
     </row>
@@ -2767,6 +2797,9 @@
       <c r="B50" s="70" t="s">
         <v>60</v>
       </c>
+      <c r="G50">
+        <v>32</v>
+      </c>
     </row>
     <row r="51" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="70">

</xml_diff>